<commit_message>
cmp 5 first letters (pdf - excel)
</commit_message>
<xml_diff>
--- a/emails/emails.xlsx
+++ b/emails/emails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Names</t>
   </si>
@@ -28,13 +28,10 @@
     <t>victorsfak@gmail.com</t>
   </si>
   <si>
-    <t>ΔΗΜΗΤΡΙΟΣ ΚΑΦΦΑΤΟΣ ΕΥΣΤΑΘΙΟΣ</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ΦΥΝΤΙΚΗΣ ΓΕΩΡΓΙΟΣ</t>
+    <t>BC ΔΗΜΗΤΡΙΟΣ ΚΑΦΦΑΤΟΣ ΕΥΣΤΑΘΙΟΣ</t>
+  </si>
+  <si>
+    <t>BC ΦΥlalalalalallaΦΥΝΤΙΚΗΣ ΓΕΩΡΓΙΟΣ</t>
   </si>
 </sst>
 </file>
@@ -84,16 +81,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -409,15 +403,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="46.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="46.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="23.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +423,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -441,21 +435,21 @@
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -465,7 +459,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -473,7 +467,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>

</xml_diff>

<commit_message>
minor changes to get undetected by google
</commit_message>
<xml_diff>
--- a/emails/emails.xlsx
+++ b/emails/emails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Names</t>
   </si>
@@ -25,13 +25,19 @@
     <t>ΧΑΤΖΗΔΑΚΙ ΣΤΥΛΙΑΝΗ</t>
   </si>
   <si>
-    <t>victorsfak@gmail.com</t>
+    <t>biktoras92@gmail.com</t>
   </si>
   <si>
     <t>BC ΔΗΜΗΤΡΙΟΣ ΚΑΦΦΑΤΟΣ ΕΥΣΤΑΘΙΟΣ</t>
   </si>
   <si>
     <t>BC ΦΥlalalalalallaΦΥΝΤΙΚΗΣ ΓΕΩΡΓΙΟΣ</t>
+  </si>
+  <si>
+    <t>victorsfak03@gmail.com</t>
+  </si>
+  <si>
+    <t>BC ΧΑΤΖΗΔΑΚΙ ΣΤΥΛΙΑΝΗ</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -460,8 +466,12 @@
       <c r="F4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>

</xml_diff>